<commit_message>
try to find valid solution
- greedy iteration
- data handler
</commit_message>
<xml_diff>
--- a/data/data_final2.xlsx
+++ b/data/data_final2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive\Document\NTHU\master\Final\HRC_taskalloc_w.TB_w.AR\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7005B5-711B-4187-9892-37E28773F1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42FD1BD4-9805-428B-9032-0E565013BE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="16305" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Therbligs1" sheetId="4" r:id="rId1"/>
@@ -266,15 +266,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -582,8 +579,8 @@
   </sheetPr>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -696,7 +693,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -705,9 +702,12 @@
       <c r="C8" t="s">
         <v>23</v>
       </c>
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -799,7 +799,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -808,9 +808,12 @@
       <c r="C16" t="s">
         <v>14</v>
       </c>
+      <c r="D16" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -926,7 +929,7 @@
   <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1583,10 +1586,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1734,7 +1737,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>45</v>
@@ -1742,19 +1745,19 @@
       <c r="C11" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>40</v>
+      <c r="A12" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>45</v>
+        <v>32</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1762,79 +1765,79 @@
         <v>9</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>9</v>
+    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>5</v>
+      <c r="E14"/>
+      <c r="F14"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15"/>
-      <c r="F15"/>
+        <v>41</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1842,10 +1845,10 @@
         <v>9</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>11</v>
@@ -1856,10 +1859,10 @@
         <v>9</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>11</v>
@@ -1867,66 +1870,66 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>5</v>
+      <c r="A22" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>21</v>
+        <v>32</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>43</v>
+        <v>32</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1934,10 +1937,10 @@
         <v>9</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>11</v>
@@ -1948,10 +1951,10 @@
         <v>9</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>11</v>
@@ -1959,35 +1962,24 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>21</v>
-      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
+      <c r="D33" s="1"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
-      <c r="D34" s="1"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
@@ -1997,10 +1989,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
+      <c r="D37" s="1"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-      <c r="D38" s="1"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
@@ -2010,10 +2002,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
+      <c r="D41" s="1"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
-      <c r="D42" s="1"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
@@ -2023,10 +2015,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
+      <c r="D45" s="1"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
-      <c r="D46" s="1"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
@@ -2036,10 +2028,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
+      <c r="D49" s="1"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
-      <c r="D50" s="1"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
@@ -2052,6 +2044,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
+      <c r="D54" s="1"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
@@ -2059,7 +2052,6 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
-      <c r="D56" s="1"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
@@ -2072,23 +2064,20 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
+      <c r="D60" s="1"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
-      <c r="D61" s="1"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
+      <c r="D63" s="1"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
-      <c r="D64" s="1"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2104,8 +2093,8 @@
   </sheetPr>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2218,7 +2207,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -2227,9 +2216,12 @@
       <c r="C8" t="s">
         <v>28</v>
       </c>
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -2321,7 +2313,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -2330,9 +2322,12 @@
       <c r="C16" t="s">
         <v>29</v>
       </c>
+      <c r="D16" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="2" t="s">

</xml_diff>

<commit_message>
add test in GASolver
</commit_message>
<xml_diff>
--- a/data/data_final2.xlsx
+++ b/data/data_final2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive\Document\NTHU\master\Final\HRC_taskalloc_w.TB_w.AR\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42FD1BD4-9805-428B-9032-0E565013BE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24736496-886D-4571-9B49-614B91111790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="16305" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Therbligs1" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="52">
   <si>
     <t>From</t>
   </si>
@@ -579,8 +579,8 @@
   </sheetPr>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -604,12 +604,8 @@
       <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -717,7 +713,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -744,8 +740,9 @@
       <c r="D11" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -755,9 +752,9 @@
       <c r="C12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -770,6 +767,8 @@
       <c r="D13" t="s">
         <v>11</v>
       </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -784,10 +783,8 @@
       <c r="D14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -797,6 +794,7 @@
       <c r="C15" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -812,7 +810,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
@@ -822,6 +820,7 @@
       <c r="C17" t="s">
         <v>14</v>
       </c>
+      <c r="D17"/>
     </row>
     <row r="18" spans="1:4" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
@@ -904,7 +903,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>5</v>
       </c>
@@ -914,6 +913,7 @@
       <c r="C24" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="D24" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2093,7 +2093,7 @@
   </sheetPr>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>

</xml_diff>